<commit_message>
Modified template and instructions.
</commit_message>
<xml_diff>
--- a/NLP/entity_dictionary__template.xlsx
+++ b/NLP/entity_dictionary__template.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3150" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="2" r:id="rId1"/>
-    <sheet name="Entities" sheetId="1" r:id="rId2"/>
+    <sheet name="ent__example" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -90,12 +90,6 @@
     <t>unc.edu</t>
   </si>
   <si>
-    <t>Note that only workbooks (.xlsx files) with a worksheet named "Entities" (case-sensitive) will be usable by the TOMES software.</t>
-  </si>
-  <si>
-    <t>The data dictionary below describes the columns in the "Entities" worksheet.</t>
-  </si>
-  <si>
     <t>Use domain-style tokens. Use only letters, periods, underscores, and hyphens.</t>
   </si>
   <si>
@@ -115,6 +109,27 @@
   </si>
   <si>
     <t>case_sensitive</t>
+  </si>
+  <si>
+    <t>The data dictionary below describes the columns in the example "ent_example" worksheet.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note that only workbooks (.xlsx files) with one or more worksheets starting with string "ent__" (case-sensitive) will be usable by the TOMES software.
+These worksheets must also contain all the columns below.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note that the string "ent__" ends with a double underscore.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -181,11 +196,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -472,42 +487,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" customWidth="1"/>
     <col min="2" max="5" width="25.7109375" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -530,24 +545,24 @@
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -587,7 +602,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
@@ -608,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -625,10 +640,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Simplified code; changed templates.
</commit_message>
<xml_diff>
--- a/NLP/entity_dictionary__template.xlsx
+++ b/NLP/entity_dictionary__template.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="2" r:id="rId1"/>
-    <sheet name="ent__example" sheetId="1" r:id="rId2"/>
+    <sheet name="Entities" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,8 +19,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Note that using nomenclature that starts with a broader concept ("FEDERAL") followed by a "." will make it easier to group/facet all sub-concepts underneath the broader concept.
+If this type of notation is used, it is highly advised to refrain from using "." characters in the remaining part of the string.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>authority</t>
   </si>
@@ -111,32 +146,18 @@
     <t>case_sensitive</t>
   </si>
   <si>
-    <t>The data dictionary below describes the columns in the example "ent_example" worksheet.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Note that only workbooks (.xlsx files) with one or more worksheets starting with string "ent__" (case-sensitive) will be usable by the TOMES software.
-These worksheets must also contain all the columns below.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note that the string "ent__" ends with a double underscore.</t>
-    </r>
+    <t>Note that only workbooks (.xlsx files) with a worksheet named "Entities" (case sensitive) will be usable by the TOMES software.
+The "Entities" worksheet must also contain all the required columns.</t>
+  </si>
+  <si>
+    <t>The data dictionary below describes the required columns for a TOMES Entity Dictionary worksheet.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +180,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -187,9 +221,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -204,6 +237,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,126 +526,126 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="2" customWidth="1"/>
-    <col min="2" max="5" width="25.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="315" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="b">
+      <c r="D7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="b">
+      <c r="E7" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -620,39 +658,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated documentation; fixed typos.
</commit_message>
<xml_diff>
--- a/NLP/entity_dictionary__template.xlsx
+++ b/NLP/entity_dictionary__template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4500" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="4950" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="2" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>Whether or not the patters should be a case-sensitive match (TRUE) or case-insensitive (FALSE).</t>
-  </si>
-  <si>
     <t>nc.gov</t>
   </si>
   <si>
@@ -111,15 +108,9 @@
     <t>A unique identifier of the institution associated with determining the pattern and label.</t>
   </si>
   <si>
-    <t>Use only letters, periods, and underscores.</t>
-  </si>
-  <si>
     <t>unc.edu</t>
   </si>
   <si>
-    <t>Use domain-style tokens. Use only letters, periods, underscores, and hyphens.</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -139,11 +130,6 @@
   </si>
   <si>
     <t>The data dictionary below describes the required columns for a TOMES Entity Dictionary worksheet.</t>
-  </si>
-  <si>
-    <t>Note that only workbooks (.xlsx files) with a worksheet named "Entities" (case sensitive) will be usable by the TOMES software.
-The "Entities" worksheet must also contain all the required columns.
-No cell in any column may be blank otherwise. The software will skip any row with a blank cell.</t>
   </si>
   <si>
     <t>Use natural language patterns and avoid punctuation marks.
@@ -152,6 +138,20 @@
 - {abc} to match only letters,
  - {123} to match only numbers,
  - {abc123} to match an alphanumeric pattern.</t>
+  </si>
+  <si>
+    <t>Note that only workbooks (.xlsx files) with a worksheet named "Entities" (case sensitive) will be usable by the TOMES software.
+The "Entities" worksheet must also contain all the required columns.
+No cell in any column may be blank. The software will skip any row with a blank cell.</t>
+  </si>
+  <si>
+    <t>Whether or not the pattern should be a case-sensitive match (TRUE) or case-insensitive (FALSE).</t>
+  </si>
+  <si>
+    <t>Use only letters, periods, underscores and hyphens.</t>
+  </si>
+  <si>
+    <t>Use domain-style tokens. Use only letters, periods, underscores and hyphens.</t>
   </si>
 </sst>
 </file>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,12 +539,12 @@
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -556,13 +556,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="315" x14ac:dyDescent="0.25">
@@ -573,41 +573,41 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="b">
         <v>1</v>
@@ -621,16 +621,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -638,16 +638,16 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -680,10 +680,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1</v>
@@ -694,36 +694,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed poor example description.
</commit_message>
<xml_diff>
--- a/NLP/entity_dictionary__template.xlsx
+++ b/NLP/entity_dictionary__template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>authority</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>A reference to the state government of North Carolina.</t>
-  </si>
-  <si>
-    <t>A simple definition of the entity that the pattern is meant to capture.</t>
   </si>
   <si>
     <t>case_sensitive</t>
@@ -134,21 +131,42 @@
     <t>FEDERAL.organization</t>
   </si>
   <si>
-    <t>FEDERAL.department</t>
-  </si>
-  <si>
-    <t>A colloquial reference to Consular Affairs at the federal Department of State.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Use only "TRUE" or "FALSE".
 Generally avoid "FALSE" unless you have a specific reason to do so (phrase is often spelled with different case). </t>
+  </si>
+  <si>
+    <t>A simple definition of the label that the pattern is meant to capture.</t>
+  </si>
+  <si>
+    <t>A reference to a federal organization, department, or agency.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,12 +189,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -205,20 +217,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -227,7 +227,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -518,121 +533,121 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="34.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="25.7109375" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="b">
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -654,61 +669,61 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="40.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="b">
+      <c r="C2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="5" t="b">
+      <c r="C3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>